<commit_message>
revise data structure documentation and outputs
</commit_message>
<xml_diff>
--- a/sampling_event/final_spreadsheets/sampling_event_protocol_data_entry_spreadsheet_marinegeo.xlsx
+++ b/sampling_event/final_spreadsheets/sampling_event_protocol_data_entry_spreadsheet_marinegeo.xlsx
@@ -71,7 +71,7 @@
     <t xml:space="preserve">SAMPLING EVENT PROTOCOL</t>
   </si>
   <si>
-    <t xml:space="preserve">DOI: 10.25573/serc.14555511.V1</t>
+    <t xml:space="preserve">DOI: 10.25573/serc.14555511.v1</t>
   </si>
   <si>
     <t xml:space="preserve">camera_used</t>
@@ -1155,7 +1155,9 @@
       <c r="B18" s="10" t="s">
         <v>47</v>
       </c>
-      <c r="C18" s="10"/>
+      <c r="C18" s="10" t="s">
+        <v>13</v>
+      </c>
       <c r="D18" s="10"/>
       <c r="E18" s="10"/>
       <c r="F18" s="10" t="s">

</xml_diff>

<commit_message>
update sampling event and envlogger protocols
</commit_message>
<xml_diff>
--- a/sampling_event/final_spreadsheets/sampling_event_protocol_data_entry_spreadsheet_marinegeo.xlsx
+++ b/sampling_event/final_spreadsheets/sampling_event_protocol_data_entry_spreadsheet_marinegeo.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <workbookPr defaultThemeVersion="166925"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="13125" windowHeight="6105" firstSheet="0" activeTab="0"/>
@@ -8,15 +8,27 @@
   <sheets>
     <sheet name="glossary" sheetId="2" state="visible" r:id="rId1"/>
     <sheet name="site metadata" sheetId="3" state="visible" r:id="rId2"/>
-    <sheet name="logger deployment" sheetId="4" state="visible" r:id="rId3"/>
-    <sheet name="transect metadata" sheetId="5" state="visible" r:id="rId4"/>
+    <sheet name="transect metadata" sheetId="4" state="visible" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+      <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="85">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="74">
   <si>
     <t>definition</t>
   </si>
@@ -71,7 +83,7 @@
     <t xml:space="preserve">SAMPLING EVENT PROTOCOL</t>
   </si>
   <si>
-    <t xml:space="preserve">DOI: 10.25573/serc.14555511.v1</t>
+    <t xml:space="preserve">DOI: 10.25573/serc.14555511.v2</t>
   </si>
   <si>
     <t xml:space="preserve">camera_used</t>
@@ -86,15 +98,6 @@
     <t xml:space="preserve">site metadata</t>
   </si>
   <si>
-    <t xml:space="preserve">deployment_location</t>
-  </si>
-  <si>
-    <t xml:space="preserve">The location of the logger at a sit, either as a latitude and longitude in decimal degrees or as a short text description, e.g. “start of transect 2”</t>
-  </si>
-  <si>
-    <t xml:space="preserve">logger deployment</t>
-  </si>
-  <si>
     <t xml:space="preserve">depth_max_m</t>
   </si>
   <si>
@@ -140,31 +143,7 @@
     <t xml:space="preserve">The name of the specific location where the sample was collected; e.g., Curlew Cay</t>
   </si>
   <si>
-    <t xml:space="preserve">site metadata, logger deployment, transect metadata</t>
-  </si>
-  <si>
-    <t xml:space="preserve">logger_deployment_notes</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Any additional notes regarding observations, context, or concerns about the logger deployment</t>
-  </si>
-  <si>
-    <t xml:space="preserve">logger_depth</t>
-  </si>
-  <si>
-    <t xml:space="preserve">The depth at which the logger is deployed</t>
-  </si>
-  <si>
-    <t xml:space="preserve">logger_identifier</t>
-  </si>
-  <si>
-    <t xml:space="preserve">A unique identifier assigned to each logger using the EnvLogger application. View the "Sampling Event Protocol" for instructions on creating IDs</t>
-  </si>
-  <si>
-    <t xml:space="preserve">logger_serial_number</t>
-  </si>
-  <si>
-    <t xml:space="preserve">The serial number associated with the logger. It can be viewed using the EnvLogger application.</t>
+    <t xml:space="preserve">site metadata, transect metadata</t>
   </si>
   <si>
     <t xml:space="preserve">photo_direction</t>
@@ -299,7 +278,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="0"/>
   <fonts count="9">
     <font>
@@ -496,6 +475,7 @@
       </fill>
     </dxf>
   </dxfs>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -853,10 +833,10 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+    <sheetView showGridLines="0" tabSelected="true" workbookViewId="0">
       <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
@@ -942,59 +922,59 @@
         <v>16</v>
       </c>
       <c r="C5" s="10" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="D5" s="10"/>
-      <c r="E5" s="10"/>
+      <c r="E5" s="10" t="s">
+        <v>18</v>
+      </c>
       <c r="F5" s="10" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="10" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="B6" s="10" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="C6" s="10" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="D6" s="10"/>
       <c r="E6" s="10" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="F6" s="10" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="B7" s="10" t="s">
         <v>23</v>
       </c>
-      <c r="B7" s="10" t="s">
-        <v>24</v>
-      </c>
       <c r="C7" s="10" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="D7" s="10"/>
-      <c r="E7" s="10" t="s">
-        <v>21</v>
-      </c>
+      <c r="E7" s="10"/>
       <c r="F7" s="10" t="s">
-        <v>22</v>
+        <v>14</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="B8" s="10" t="s">
         <v>25</v>
       </c>
-      <c r="B8" s="10" t="s">
-        <v>26</v>
-      </c>
       <c r="C8" s="10" t="s">
-        <v>20</v>
+        <v>13</v>
       </c>
       <c r="D8" s="10"/>
       <c r="E8" s="10"/>
@@ -1004,10 +984,10 @@
     </row>
     <row r="9">
       <c r="A9" s="10" t="s">
+        <v>26</v>
+      </c>
+      <c r="B9" s="10" t="s">
         <v>27</v>
-      </c>
-      <c r="B9" s="10" t="s">
-        <v>28</v>
       </c>
       <c r="C9" s="10" t="s">
         <v>13</v>
@@ -1020,10 +1000,10 @@
     </row>
     <row r="10">
       <c r="A10" s="10" t="s">
+        <v>28</v>
+      </c>
+      <c r="B10" s="10" t="s">
         <v>29</v>
-      </c>
-      <c r="B10" s="10" t="s">
-        <v>30</v>
       </c>
       <c r="C10" s="10" t="s">
         <v>13</v>
@@ -1031,7 +1011,7 @@
       <c r="D10" s="10"/>
       <c r="E10" s="10"/>
       <c r="F10" s="10" t="s">
-        <v>14</v>
+        <v>30</v>
       </c>
     </row>
     <row r="11">
@@ -1042,20 +1022,20 @@
         <v>32</v>
       </c>
       <c r="C11" s="10" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="D11" s="10"/>
       <c r="E11" s="10"/>
       <c r="F11" s="10" t="s">
-        <v>33</v>
+        <v>14</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="10" t="s">
+        <v>33</v>
+      </c>
+      <c r="B12" s="10" t="s">
         <v>34</v>
-      </c>
-      <c r="B12" s="10" t="s">
-        <v>35</v>
       </c>
       <c r="C12" s="10" t="s">
         <v>13</v>
@@ -1063,33 +1043,31 @@
       <c r="D12" s="10"/>
       <c r="E12" s="10"/>
       <c r="F12" s="10" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="10" t="s">
+        <v>35</v>
+      </c>
+      <c r="B13" s="10" t="s">
         <v>36</v>
       </c>
-      <c r="B13" s="10" t="s">
-        <v>37</v>
-      </c>
       <c r="C13" s="10" t="s">
-        <v>20</v>
+        <v>13</v>
       </c>
       <c r="D13" s="10"/>
-      <c r="E13" s="10" t="s">
-        <v>21</v>
-      </c>
+      <c r="E13" s="10"/>
       <c r="F13" s="10" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="10" t="s">
+        <v>37</v>
+      </c>
+      <c r="B14" s="10" t="s">
         <v>38</v>
-      </c>
-      <c r="B14" s="10" t="s">
-        <v>39</v>
       </c>
       <c r="C14" s="10" t="s">
         <v>13</v>
@@ -1097,36 +1075,38 @@
       <c r="D14" s="10"/>
       <c r="E14" s="10"/>
       <c r="F14" s="10" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="10" t="s">
+        <v>39</v>
+      </c>
+      <c r="B15" s="10" t="s">
         <v>40</v>
       </c>
-      <c r="B15" s="10" t="s">
-        <v>41</v>
-      </c>
       <c r="C15" s="10" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="D15" s="10"/>
       <c r="E15" s="10"/>
       <c r="F15" s="10" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" s="10" t="s">
+        <v>41</v>
+      </c>
+      <c r="B16" s="10" t="s">
         <v>42</v>
       </c>
-      <c r="B16" s="10" t="s">
+      <c r="C16" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="D16" s="10" t="s">
         <v>43</v>
       </c>
-      <c r="C16" s="10" t="s">
-        <v>20</v>
-      </c>
-      <c r="D16" s="10"/>
       <c r="E16" s="10"/>
       <c r="F16" s="10" t="s">
         <v>14</v>
@@ -1140,9 +1120,11 @@
         <v>45</v>
       </c>
       <c r="C17" s="10" t="s">
-        <v>13</v>
-      </c>
-      <c r="D17" s="10"/>
+        <v>17</v>
+      </c>
+      <c r="D17" s="10" t="s">
+        <v>46</v>
+      </c>
       <c r="E17" s="10"/>
       <c r="F17" s="10" t="s">
         <v>14</v>
@@ -1150,15 +1132,17 @@
     </row>
     <row r="18">
       <c r="A18" s="10" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="B18" s="10" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="C18" s="10" t="s">
-        <v>13</v>
-      </c>
-      <c r="D18" s="10"/>
+        <v>17</v>
+      </c>
+      <c r="D18" s="10" t="s">
+        <v>49</v>
+      </c>
       <c r="E18" s="10"/>
       <c r="F18" s="10" t="s">
         <v>14</v>
@@ -1166,10 +1150,10 @@
     </row>
     <row r="19">
       <c r="A19" s="10" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="B19" s="10" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="C19" s="10" t="s">
         <v>13</v>
@@ -1182,72 +1166,68 @@
     </row>
     <row r="20">
       <c r="A20" s="10" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="B20" s="10" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="C20" s="10" t="s">
-        <v>20</v>
-      </c>
-      <c r="D20" s="10"/>
+        <v>13</v>
+      </c>
+      <c r="D20" s="10" t="s">
+        <v>54</v>
+      </c>
       <c r="E20" s="10"/>
       <c r="F20" s="10" t="s">
-        <v>14</v>
+        <v>30</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" s="10" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="B21" s="10" t="s">
-        <v>53</v>
+        <v>56</v>
       </c>
       <c r="C21" s="10" t="s">
-        <v>20</v>
-      </c>
-      <c r="D21" s="10" t="s">
-        <v>54</v>
-      </c>
+        <v>13</v>
+      </c>
+      <c r="D21" s="10"/>
       <c r="E21" s="10"/>
       <c r="F21" s="10" t="s">
-        <v>33</v>
+        <v>14</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" s="10" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="B22" s="10" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="C22" s="10" t="s">
-        <v>20</v>
-      </c>
-      <c r="D22" s="10" t="s">
-        <v>57</v>
-      </c>
+        <v>17</v>
+      </c>
+      <c r="D22" s="10"/>
       <c r="E22" s="10"/>
       <c r="F22" s="10" t="s">
-        <v>33</v>
+        <v>14</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" s="10" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="B23" s="10" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="C23" s="10" t="s">
-        <v>20</v>
-      </c>
-      <c r="D23" s="10" t="s">
-        <v>60</v>
-      </c>
+        <v>17</v>
+      </c>
+      <c r="D23" s="10"/>
       <c r="E23" s="10"/>
       <c r="F23" s="10" t="s">
-        <v>33</v>
+        <v>19</v>
       </c>
     </row>
     <row r="24">
@@ -1258,62 +1238,68 @@
         <v>62</v>
       </c>
       <c r="C24" s="10" t="s">
-        <v>13</v>
-      </c>
-      <c r="D24" s="10"/>
+        <v>17</v>
+      </c>
+      <c r="D24" s="10" t="s">
+        <v>63</v>
+      </c>
       <c r="E24" s="10"/>
       <c r="F24" s="10" t="s">
-        <v>14</v>
+        <v>19</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" s="10" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="B25" s="10" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="C25" s="10" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="D25" s="10" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="E25" s="10"/>
       <c r="F25" s="10" t="s">
-        <v>33</v>
+        <v>19</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" s="10" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="B26" s="10" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="C26" s="10" t="s">
-        <v>13</v>
-      </c>
-      <c r="D26" s="10"/>
+        <v>17</v>
+      </c>
+      <c r="D26" s="10" t="s">
+        <v>63</v>
+      </c>
       <c r="E26" s="10"/>
       <c r="F26" s="10" t="s">
-        <v>14</v>
+        <v>19</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" s="10" t="s">
+        <v>69</v>
+      </c>
+      <c r="B27" s="10" t="s">
         <v>68</v>
       </c>
-      <c r="B27" s="10" t="s">
-        <v>69</v>
-      </c>
       <c r="C27" s="10" t="s">
-        <v>20</v>
-      </c>
-      <c r="D27" s="10"/>
+        <v>17</v>
+      </c>
+      <c r="D27" s="10" t="s">
+        <v>66</v>
+      </c>
       <c r="E27" s="10"/>
       <c r="F27" s="10" t="s">
-        <v>14</v>
+        <v>19</v>
       </c>
     </row>
     <row r="28">
@@ -1324,12 +1310,12 @@
         <v>71</v>
       </c>
       <c r="C28" s="10" t="s">
-        <v>20</v>
+        <v>13</v>
       </c>
       <c r="D28" s="10"/>
       <c r="E28" s="10"/>
       <c r="F28" s="10" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
     </row>
     <row r="29">
@@ -1339,110 +1325,22 @@
       <c r="B29" s="10" t="s">
         <v>73</v>
       </c>
-      <c r="C29" s="10" t="s">
-        <v>20</v>
-      </c>
-      <c r="D29" s="10" t="s">
-        <v>74</v>
-      </c>
-      <c r="E29" s="10"/>
+      <c r="C29" s="10"/>
+      <c r="D29" s="10"/>
+      <c r="E29" s="10" t="s">
+        <v>18</v>
+      </c>
       <c r="F29" s="10" t="s">
-        <v>22</v>
+        <v>14</v>
       </c>
     </row>
     <row r="30">
-      <c r="A30" s="10" t="s">
-        <v>75</v>
-      </c>
-      <c r="B30" s="10" t="s">
-        <v>76</v>
-      </c>
-      <c r="C30" s="10" t="s">
-        <v>20</v>
-      </c>
-      <c r="D30" s="10" t="s">
-        <v>77</v>
-      </c>
-      <c r="E30" s="10"/>
-      <c r="F30" s="10" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="31">
-      <c r="A31" s="10" t="s">
-        <v>78</v>
-      </c>
-      <c r="B31" s="10" t="s">
-        <v>79</v>
-      </c>
-      <c r="C31" s="10" t="s">
-        <v>20</v>
-      </c>
-      <c r="D31" s="10" t="s">
-        <v>74</v>
-      </c>
-      <c r="E31" s="10"/>
-      <c r="F31" s="10" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="32">
-      <c r="A32" s="10" t="s">
-        <v>80</v>
-      </c>
-      <c r="B32" s="10" t="s">
-        <v>79</v>
-      </c>
-      <c r="C32" s="10" t="s">
-        <v>20</v>
-      </c>
-      <c r="D32" s="10" t="s">
-        <v>77</v>
-      </c>
-      <c r="E32" s="10"/>
-      <c r="F32" s="10" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="33">
-      <c r="A33" s="10" t="s">
-        <v>81</v>
-      </c>
-      <c r="B33" s="10" t="s">
-        <v>82</v>
-      </c>
-      <c r="C33" s="10" t="s">
-        <v>13</v>
-      </c>
-      <c r="D33" s="10"/>
-      <c r="E33" s="10"/>
-      <c r="F33" s="10" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="34">
-      <c r="A34" s="10" t="s">
-        <v>83</v>
-      </c>
-      <c r="B34" s="10" t="s">
-        <v>84</v>
-      </c>
-      <c r="C34" s="10"/>
-      <c r="D34" s="10"/>
-      <c r="E34" s="10" t="s">
-        <v>21</v>
-      </c>
-      <c r="F34" s="10" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="35">
-      <c r="A35" s="11"/>
-      <c r="B35" s="11"/>
-      <c r="C35" s="11"/>
-      <c r="D35" s="11"/>
-      <c r="E35" s="11"/>
-      <c r="F35" s="11"/>
+      <c r="A30" s="11"/>
+      <c r="B30" s="11"/>
+      <c r="C30" s="11"/>
+      <c r="D30" s="11"/>
+      <c r="E30" s="11"/>
+      <c r="F30" s="11"/>
     </row>
   </sheetData>
   <mergeCells count="3">
@@ -1467,10 +1365,10 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0" zoomScale="100" showGridLines="1" tabSelected="0"/>
+    <sheetView workbookViewId="0" zoomScale="100" showGridLines="1" tabSelected="false"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.0" baseColWidth="10"/>
   <cols>
@@ -1496,58 +1394,58 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="12" t="s">
-        <v>63</v>
+        <v>52</v>
       </c>
       <c r="B1" s="12" t="s">
+        <v>28</v>
+      </c>
+      <c r="C1" s="12" t="s">
+        <v>47</v>
+      </c>
+      <c r="D1" s="12" t="s">
+        <v>44</v>
+      </c>
+      <c r="E1" s="12" t="s">
+        <v>41</v>
+      </c>
+      <c r="F1" s="12" t="s">
+        <v>72</v>
+      </c>
+      <c r="G1" s="12" t="s">
+        <v>26</v>
+      </c>
+      <c r="H1" s="12" t="s">
+        <v>57</v>
+      </c>
+      <c r="I1" s="12" t="s">
+        <v>39</v>
+      </c>
+      <c r="J1" s="12" t="s">
+        <v>22</v>
+      </c>
+      <c r="K1" s="12" t="s">
+        <v>24</v>
+      </c>
+      <c r="L1" s="12" t="s">
+        <v>50</v>
+      </c>
+      <c r="M1" s="12" t="s">
+        <v>33</v>
+      </c>
+      <c r="N1" s="12" t="s">
+        <v>35</v>
+      </c>
+      <c r="O1" s="12" t="s">
         <v>31</v>
-      </c>
-      <c r="C1" s="12" t="s">
-        <v>58</v>
-      </c>
-      <c r="D1" s="12" t="s">
-        <v>55</v>
-      </c>
-      <c r="E1" s="12" t="s">
-        <v>52</v>
-      </c>
-      <c r="F1" s="12" t="s">
-        <v>83</v>
-      </c>
-      <c r="G1" s="12" t="s">
-        <v>29</v>
-      </c>
-      <c r="H1" s="12" t="s">
-        <v>68</v>
-      </c>
-      <c r="I1" s="12" t="s">
-        <v>50</v>
-      </c>
-      <c r="J1" s="12" t="s">
-        <v>25</v>
-      </c>
-      <c r="K1" s="12" t="s">
-        <v>27</v>
-      </c>
-      <c r="L1" s="12" t="s">
-        <v>61</v>
-      </c>
-      <c r="M1" s="12" t="s">
-        <v>44</v>
-      </c>
-      <c r="N1" s="12" t="s">
-        <v>46</v>
-      </c>
-      <c r="O1" s="12" t="s">
-        <v>42</v>
       </c>
       <c r="P1" s="12" t="s">
         <v>11</v>
       </c>
       <c r="Q1" s="12" t="s">
-        <v>48</v>
+        <v>37</v>
       </c>
       <c r="R1" s="12" t="s">
-        <v>66</v>
+        <v>55</v>
       </c>
     </row>
   </sheetData>
@@ -1557,125 +1455,55 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0" zoomScale="100" showGridLines="1" tabSelected="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.0" baseColWidth="10"/>
-  <cols>
-    <col min="1" max="1" width="9.71" hidden="0" customWidth="1"/>
-    <col min="2" max="2" width="13.71" hidden="0" customWidth="1"/>
-    <col min="3" max="3" width="22.71" hidden="0" customWidth="1"/>
-    <col min="4" max="4" width="23.71" hidden="0" customWidth="1"/>
-    <col min="5" max="5" width="21.71" hidden="0" customWidth="1"/>
-    <col min="6" max="6" width="17.71" hidden="0" customWidth="1"/>
-    <col min="7" max="7" width="20.71" hidden="0" customWidth="1"/>
-    <col min="8" max="8" width="12.71" hidden="0" customWidth="1"/>
-    <col min="9" max="9" width="19.71" hidden="0" customWidth="1"/>
-    <col min="10" max="10" width="23.71" hidden="0" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1">
-      <c r="A1" s="12" t="s">
-        <v>63</v>
-      </c>
-      <c r="B1" s="12" t="s">
-        <v>31</v>
-      </c>
-      <c r="C1" s="12" t="s">
-        <v>58</v>
-      </c>
-      <c r="D1" s="12" t="s">
-        <v>55</v>
-      </c>
-      <c r="E1" s="12" t="s">
-        <v>52</v>
-      </c>
-      <c r="F1" s="12" t="s">
-        <v>38</v>
-      </c>
-      <c r="G1" s="12" t="s">
-        <v>40</v>
-      </c>
-      <c r="H1" s="12" t="s">
-        <v>36</v>
-      </c>
-      <c r="I1" s="12" t="s">
-        <v>15</v>
-      </c>
-      <c r="J1" s="12" t="s">
-        <v>34</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0" zoomScale="100" showGridLines="1" tabSelected="0"/>
+    <sheetView workbookViewId="0" zoomScale="100" showGridLines="1" tabSelected="false"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.0" baseColWidth="10"/>
   <cols>
     <col min="1" max="1" width="9.71" hidden="0" customWidth="1"/>
     <col min="2" max="2" width="13.71" hidden="0" customWidth="1"/>
     <col min="3" max="3" width="8.71" hidden="0" customWidth="1"/>
-    <col min="4" max="4" width="22.71" hidden="0" customWidth="1"/>
-    <col min="5" max="5" width="23.71" hidden="0" customWidth="1"/>
-    <col min="6" max="6" width="21.71" hidden="0" customWidth="1"/>
-    <col min="7" max="7" width="31.71" hidden="0" customWidth="1"/>
-    <col min="8" max="8" width="32.71" hidden="0" customWidth="1"/>
-    <col min="9" max="9" width="29.71" hidden="0" customWidth="1"/>
-    <col min="10" max="10" width="30.71" hidden="0" customWidth="1"/>
-    <col min="11" max="11" width="11.71" hidden="0" customWidth="1"/>
-    <col min="12" max="12" width="11.71" hidden="0" customWidth="1"/>
-    <col min="13" max="13" width="14.71" hidden="0" customWidth="1"/>
+    <col min="4" max="4" width="31.71" hidden="0" customWidth="1"/>
+    <col min="5" max="5" width="32.71" hidden="0" customWidth="1"/>
+    <col min="6" max="6" width="29.71" hidden="0" customWidth="1"/>
+    <col min="7" max="7" width="30.71" hidden="0" customWidth="1"/>
+    <col min="8" max="8" width="11.71" hidden="0" customWidth="1"/>
+    <col min="9" max="9" width="11.71" hidden="0" customWidth="1"/>
+    <col min="10" max="10" width="14.71" hidden="0" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1">
       <c r="A1" s="12" t="s">
-        <v>63</v>
+        <v>52</v>
       </c>
       <c r="B1" s="12" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="C1" s="12" t="s">
+        <v>59</v>
+      </c>
+      <c r="D1" s="12" t="s">
+        <v>61</v>
+      </c>
+      <c r="E1" s="12" t="s">
+        <v>64</v>
+      </c>
+      <c r="F1" s="12" t="s">
+        <v>67</v>
+      </c>
+      <c r="G1" s="12" t="s">
+        <v>69</v>
+      </c>
+      <c r="H1" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="I1" s="12" t="s">
+        <v>15</v>
+      </c>
+      <c r="J1" s="12" t="s">
         <v>70</v>
-      </c>
-      <c r="D1" s="12" t="s">
-        <v>58</v>
-      </c>
-      <c r="E1" s="12" t="s">
-        <v>55</v>
-      </c>
-      <c r="F1" s="12" t="s">
-        <v>52</v>
-      </c>
-      <c r="G1" s="12" t="s">
-        <v>72</v>
-      </c>
-      <c r="H1" s="12" t="s">
-        <v>75</v>
-      </c>
-      <c r="I1" s="12" t="s">
-        <v>78</v>
-      </c>
-      <c r="J1" s="12" t="s">
-        <v>80</v>
-      </c>
-      <c r="K1" s="12" t="s">
-        <v>23</v>
-      </c>
-      <c r="L1" s="12" t="s">
-        <v>18</v>
-      </c>
-      <c r="M1" s="12" t="s">
-        <v>81</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
update sampling event protocol
</commit_message>
<xml_diff>
--- a/sampling_event/final_spreadsheets/sampling_event_protocol_data_entry_spreadsheet_marinegeo.xlsx
+++ b/sampling_event/final_spreadsheets/sampling_event_protocol_data_entry_spreadsheet_marinegeo.xlsx
@@ -83,7 +83,7 @@
     <t xml:space="preserve">SAMPLING EVENT PROTOCOL</t>
   </si>
   <si>
-    <t xml:space="preserve">DOI: 10.25573/serc.14555511.v2</t>
+    <t xml:space="preserve">DOI: 10.25573/serc.14555511.v3</t>
   </si>
   <si>
     <t xml:space="preserve">camera_used</t>
@@ -1109,7 +1109,7 @@
       </c>
       <c r="E16" s="10"/>
       <c r="F16" s="10" t="s">
-        <v>14</v>
+        <v>30</v>
       </c>
     </row>
     <row r="17">
@@ -1127,7 +1127,7 @@
       </c>
       <c r="E17" s="10"/>
       <c r="F17" s="10" t="s">
-        <v>14</v>
+        <v>30</v>
       </c>
     </row>
     <row r="18">
@@ -1145,7 +1145,7 @@
       </c>
       <c r="E18" s="10"/>
       <c r="F18" s="10" t="s">
-        <v>14</v>
+        <v>30</v>
       </c>
     </row>
     <row r="19">
@@ -1465,13 +1465,16 @@
     <col min="1" max="1" width="9.71" hidden="0" customWidth="1"/>
     <col min="2" max="2" width="13.71" hidden="0" customWidth="1"/>
     <col min="3" max="3" width="8.71" hidden="0" customWidth="1"/>
-    <col min="4" max="4" width="31.71" hidden="0" customWidth="1"/>
-    <col min="5" max="5" width="32.71" hidden="0" customWidth="1"/>
-    <col min="6" max="6" width="29.71" hidden="0" customWidth="1"/>
-    <col min="7" max="7" width="30.71" hidden="0" customWidth="1"/>
-    <col min="8" max="8" width="11.71" hidden="0" customWidth="1"/>
-    <col min="9" max="9" width="11.71" hidden="0" customWidth="1"/>
-    <col min="10" max="10" width="14.71" hidden="0" customWidth="1"/>
+    <col min="4" max="4" width="22.71" hidden="0" customWidth="1"/>
+    <col min="5" max="5" width="23.71" hidden="0" customWidth="1"/>
+    <col min="6" max="6" width="21.71" hidden="0" customWidth="1"/>
+    <col min="7" max="7" width="31.71" hidden="0" customWidth="1"/>
+    <col min="8" max="8" width="32.71" hidden="0" customWidth="1"/>
+    <col min="9" max="9" width="29.71" hidden="0" customWidth="1"/>
+    <col min="10" max="10" width="30.71" hidden="0" customWidth="1"/>
+    <col min="11" max="11" width="11.71" hidden="0" customWidth="1"/>
+    <col min="12" max="12" width="11.71" hidden="0" customWidth="1"/>
+    <col min="13" max="13" width="14.71" hidden="0" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -1485,24 +1488,33 @@
         <v>59</v>
       </c>
       <c r="D1" s="12" t="s">
+        <v>47</v>
+      </c>
+      <c r="E1" s="12" t="s">
+        <v>44</v>
+      </c>
+      <c r="F1" s="12" t="s">
+        <v>41</v>
+      </c>
+      <c r="G1" s="12" t="s">
         <v>61</v>
       </c>
-      <c r="E1" s="12" t="s">
+      <c r="H1" s="12" t="s">
         <v>64</v>
       </c>
-      <c r="F1" s="12" t="s">
+      <c r="I1" s="12" t="s">
         <v>67</v>
       </c>
-      <c r="G1" s="12" t="s">
+      <c r="J1" s="12" t="s">
         <v>69</v>
       </c>
-      <c r="H1" s="12" t="s">
+      <c r="K1" s="12" t="s">
         <v>20</v>
       </c>
-      <c r="I1" s="12" t="s">
+      <c r="L1" s="12" t="s">
         <v>15</v>
       </c>
-      <c r="J1" s="12" t="s">
+      <c r="M1" s="12" t="s">
         <v>70</v>
       </c>
     </row>

</xml_diff>